<commit_message>
Alteração na planilha de requisitos
</commit_message>
<xml_diff>
--- a/Documentação/Sprint1/requisitos.xlsx
+++ b/Documentação/Sprint1/requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\monitor.me\Documentação\Sprint1\Negócios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\monitor.me\Documentação\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770903D1-132B-4734-A6D3-A14A44639693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90D4BBD-CDF2-4273-A4A6-6C6C8B4596CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="120">
-  <si>
-    <t>Proposto</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="127">
   <si>
     <t>Solicitante</t>
   </si>
@@ -244,6 +241,288 @@
     <t>Dependências Externas entre Requisitos (Rastreabilidade)</t>
   </si>
   <si>
+    <t>Projeto: Monitor.Me</t>
+  </si>
+  <si>
+    <t>Cada usuário terá um cadastro para cadastrar seus hardwares.</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>A aplicação deverá possuir tela de cadastro de usuários.</t>
+  </si>
+  <si>
+    <t>Cadastramento de hardwares e  seus respectivos componentes.</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>A aplicação deverá possuir cadastro de CPU.</t>
+  </si>
+  <si>
+    <t>A aplicação deverá possuir cadastro de RAM.</t>
+  </si>
+  <si>
+    <t>A aplicação deverá possuir cadastro de GPU.</t>
+  </si>
+  <si>
+    <t>A aplicação deverá possuir cadastro de HD.</t>
+  </si>
+  <si>
+    <t>Cadastro e edição de CPU.</t>
+  </si>
+  <si>
+    <t>Cadastro e edição de RAM.</t>
+  </si>
+  <si>
+    <t>Cadastro e edição de GPU</t>
+  </si>
+  <si>
+    <t>Cadastro e edição de HD.</t>
+  </si>
+  <si>
+    <t>Banco de Dados armazenado na Nuvem</t>
+  </si>
+  <si>
+    <t>Dados da aplicação enviados diretamente para a nuvem.</t>
+  </si>
+  <si>
+    <t>Modelagem lógica do banco de dados SQL</t>
+  </si>
+  <si>
+    <t>Script de criação de tabelas e inserção de dados</t>
+  </si>
+  <si>
+    <t>Criação e hospedagem do banco de dados na nuvem</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>Modelar o banco de dados de acordo com os dados e relacionamentos necessários.</t>
+  </si>
+  <si>
+    <t>Script para criar as tabelas e inserir dados no banco.</t>
+  </si>
+  <si>
+    <t>Criar e hospedar banco de dados em um serviço da nuvem.</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>O cadastro de usuários deverá ser feito pelo preenchimento de formulário.</t>
+  </si>
+  <si>
+    <t>Os campos do formulário necessitam de validação.</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Criação de cadastro do usuário.</t>
+  </si>
+  <si>
+    <t>Validação dos campos de cadastro.</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Suporte ao usuário</t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk integrada na página web</t>
+  </si>
+  <si>
+    <t>Envio de notificações para o usuário</t>
+  </si>
+  <si>
+    <t>Emissão de alertas para o usuário.</t>
+  </si>
+  <si>
+    <t>Conexão de todos os formulários e registros de usuário e hardware com o BD</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Oferecer suporte online ao usuário</t>
+  </si>
+  <si>
+    <t>Armazenar todos os registros de usuários e componentes.</t>
+  </si>
+  <si>
+    <t>Gerson</t>
+  </si>
+  <si>
+    <t>Notificações push utilizando o Slack</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Login e Logout de usuário</t>
+  </si>
+  <si>
+    <t>Página com campos de login</t>
+  </si>
+  <si>
+    <t>Validação do formulário de login</t>
+  </si>
+  <si>
+    <t>Botão para fazer logout</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>Página para o usuário realizar seu login</t>
+  </si>
+  <si>
+    <t>Validação dos campos de login.</t>
+  </si>
+  <si>
+    <t>Opção de logout nas telas do site quando o usuário está logado.</t>
+  </si>
+  <si>
+    <t>Realização de cadastro de usuário pelo sistema</t>
+  </si>
+  <si>
+    <t>Campos de formulário na página de cadastro</t>
+  </si>
+  <si>
+    <t>Verificar e validas os campos de cadastro</t>
+  </si>
+  <si>
+    <t>A aplicação deverá possuir tela de cadastro de componentes.</t>
+  </si>
+  <si>
+    <t>Cadastro de componentes no sistema.</t>
+  </si>
+  <si>
+    <t>Cadastro de CPU no sistema.</t>
+  </si>
+  <si>
+    <t>Cadastro de RAM no sistema.</t>
+  </si>
+  <si>
+    <t>Cadastro de GPU no sistema.</t>
+  </si>
+  <si>
+    <t>Cadastro de HD no sistema.</t>
+  </si>
+  <si>
+    <t>Banco de Dados SQL da aplicação hospedado na Azure</t>
+  </si>
+  <si>
+    <t>Modelagem lógica realizada e validada pelo solicitante.</t>
+  </si>
+  <si>
+    <t>Tabelas criadas e dados inseridos através do script</t>
+  </si>
+  <si>
+    <t>Criar o banco em um serviço cloud</t>
+  </si>
+  <si>
+    <t>Realizar conexão de todos os registros do sistema com o BD</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>Help desk integrado e funcionando no site</t>
+  </si>
+  <si>
+    <t>Página de login do usuário, botão de logout</t>
+  </si>
+  <si>
+    <t>Página de login do usuário conectada com o BD</t>
+  </si>
+  <si>
+    <t>Validação dos campos do formulário</t>
+  </si>
+  <si>
+    <t>Botão de logout nas páginas do usuário logado.</t>
+  </si>
+  <si>
+    <t>Envio de notificações para o usuário via Slack</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Guilherme</t>
+  </si>
+  <si>
+    <t>Igor</t>
+  </si>
+  <si>
+    <t>Fernanda</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
+    <r>
+      <t>Autor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Exo 2"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <rFont val="Exo 2"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Bruno Ladislau</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>Data</t>
     </r>
@@ -256,260 +535,22 @@
       </rPr>
       <t xml:space="preserve">:  </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>Autor</t>
-    </r>
     <r>
       <rPr>
+        <b/>
         <sz val="10"/>
-        <color indexed="8"/>
+        <color theme="0"/>
         <rFont val="Exo 2"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">: </t>
+      <t>14/02/2020</t>
     </r>
   </si>
   <si>
-    <t>Projeto: Monitor.Me</t>
-  </si>
-  <si>
-    <t>Cada usuário terá um cadastro para cadastrar seus hardwares.</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Essencial</t>
-  </si>
-  <si>
-    <t>A aplicação deverá possuir tela de cadastro de usuários.</t>
-  </si>
-  <si>
-    <t>Cadastramento de hardwares e  seus respectivos componentes.</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>A aplicação deverá possuir cadastro de CPU.</t>
-  </si>
-  <si>
-    <t>A aplicação deverá possuir cadastro de RAM.</t>
-  </si>
-  <si>
-    <t>A aplicação deverá possuir cadastro de GPU.</t>
-  </si>
-  <si>
-    <t>A aplicação deverá possuir cadastro de HD.</t>
-  </si>
-  <si>
-    <t>Cadastro e edição de CPU.</t>
-  </si>
-  <si>
-    <t>Cadastro e edição de RAM.</t>
-  </si>
-  <si>
-    <t>Cadastro e edição de GPU</t>
-  </si>
-  <si>
-    <t>Cadastro e edição de HD.</t>
-  </si>
-  <si>
-    <t>Banco de Dados armazenado na Nuvem</t>
-  </si>
-  <si>
-    <t>Dados da aplicação enviados diretamente para a nuvem.</t>
-  </si>
-  <si>
-    <t>Modelagem lógica do banco de dados SQL</t>
-  </si>
-  <si>
-    <t>Script de criação de tabelas e inserção de dados</t>
-  </si>
-  <si>
-    <t>Criação e hospedagem do banco de dados na nuvem</t>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>3.2</t>
-  </si>
-  <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>Modelar o banco de dados de acordo com os dados e relacionamentos necessários.</t>
-  </si>
-  <si>
-    <t>Script para criar as tabelas e inserir dados no banco.</t>
-  </si>
-  <si>
-    <t>Criar e hospedar banco de dados em um serviço da nuvem.</t>
-  </si>
-  <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>Baixa</t>
-  </si>
-  <si>
-    <t>3.4</t>
-  </si>
-  <si>
-    <t>O cadastro de usuários deverá ser feito pelo preenchimento de formulário.</t>
-  </si>
-  <si>
-    <t>Os campos do formulário necessitam de validação.</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>Criação de cadastro do usuário.</t>
-  </si>
-  <si>
-    <t>Validação dos campos de cadastro.</t>
-  </si>
-  <si>
-    <t>Importante</t>
-  </si>
-  <si>
-    <t>Suporte ao usuário</t>
-  </si>
-  <si>
-    <t>Ferramenta de Help Desk integrada na página web</t>
-  </si>
-  <si>
-    <t>Envio de notificações para o usuário</t>
-  </si>
-  <si>
-    <t>Emissão de alertas para o usuário.</t>
-  </si>
-  <si>
-    <t>Conexão de todos os formulários e registros de usuário e hardware com o BD</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>Oferecer suporte online ao usuário</t>
-  </si>
-  <si>
-    <t>Armazenar todos os registros de usuários e componentes.</t>
-  </si>
-  <si>
-    <t>Gerson</t>
-  </si>
-  <si>
-    <t>Notificações push utilizando o Slack</t>
-  </si>
-  <si>
-    <t>5.1</t>
-  </si>
-  <si>
-    <t>Login e Logout de usuário</t>
-  </si>
-  <si>
-    <t>Página com campos de login</t>
-  </si>
-  <si>
-    <t>Validação do formulário de login</t>
-  </si>
-  <si>
-    <t>Botão para fazer logout</t>
-  </si>
-  <si>
-    <t>6.1</t>
-  </si>
-  <si>
-    <t>6.2</t>
-  </si>
-  <si>
-    <t>6.3</t>
-  </si>
-  <si>
-    <t>Página para o usuário realizar seu login</t>
-  </si>
-  <si>
-    <t>Validação dos campos de login.</t>
-  </si>
-  <si>
-    <t>Opção de logout nas telas do site quando o usuário está logado.</t>
-  </si>
-  <si>
-    <t>Realização de cadastro de usuário pelo sistema</t>
-  </si>
-  <si>
-    <t>Campos de formulário na página de cadastro</t>
-  </si>
-  <si>
-    <t>Verificar e validas os campos de cadastro</t>
-  </si>
-  <si>
-    <t>A aplicação deverá possuir tela de cadastro de componentes.</t>
-  </si>
-  <si>
-    <t>Cadastro de componentes no sistema.</t>
-  </si>
-  <si>
-    <t>Cadastro de CPU no sistema.</t>
-  </si>
-  <si>
-    <t>Cadastro de RAM no sistema.</t>
-  </si>
-  <si>
-    <t>Cadastro de GPU no sistema.</t>
-  </si>
-  <si>
-    <t>Cadastro de HD no sistema.</t>
-  </si>
-  <si>
-    <t>Banco de Dados SQL da aplicação hospedado na Azure</t>
-  </si>
-  <si>
-    <t>Modelagem lógica realizada e validada pelo solicitante.</t>
-  </si>
-  <si>
-    <t>Tabelas criadas e dados inseridos através do script</t>
-  </si>
-  <si>
-    <t>Criar o banco em um serviço cloud</t>
-  </si>
-  <si>
-    <t>Realizar conexão de todos os registros do sistema com o BD</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>1.0.1</t>
-  </si>
-  <si>
-    <t>1.0.2</t>
-  </si>
-  <si>
-    <t>Help desk integrado e funcionando no site</t>
-  </si>
-  <si>
-    <t>Página de login do usuário, botão de logout</t>
-  </si>
-  <si>
-    <t>Página de login do usuário conectada com o BD</t>
-  </si>
-  <si>
-    <t>Validação dos campos do formulário</t>
-  </si>
-  <si>
-    <t>Botão de logout nas páginas do usuário logado.</t>
-  </si>
-  <si>
-    <t>Envio de notificações para o usuário via Slack</t>
+    <t>Site institucional  responsivo contruído em Angular</t>
+  </si>
+  <si>
+    <t>SPA institucional</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1206,9 +1247,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1733,7 +1771,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2199216</xdr:colOff>
+      <xdr:colOff>1940680</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -2154,33 +2192,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B2" s="64" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="B2" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
     </row>
     <row r="4" spans="2:5" ht="27" customHeight="1">
       <c r="B4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15">
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -2229,7 +2267,7 @@
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E37" s="3">
         <v>41293</v>
@@ -2237,12 +2275,12 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="15" customHeight="1">
       <c r="B39" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2258,18 +2296,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:V77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="7" customWidth="1"/>
     <col min="4" max="4" width="37.28515625" style="7" customWidth="1"/>
     <col min="5" max="5" width="29.140625" style="7" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="7" customWidth="1"/>
@@ -2305,72 +2343,72 @@
       <c r="Q1" s="12"/>
       <c r="R1" s="13"/>
       <c r="S1" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U1" s="12"/>
     </row>
     <row r="2" spans="2:22" ht="16.5" customHeight="1" thickBot="1">
-      <c r="E2" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="80"/>
+      <c r="E2" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="79" t="s">
+        <v>124</v>
+      </c>
+      <c r="P2" s="79"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="16"/>
       <c r="T2" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U2" s="12"/>
     </row>
     <row r="3" spans="2:22" ht="14.25" customHeight="1" thickBot="1">
-      <c r="E3" s="77"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="82"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="81"/>
       <c r="Q3" s="7"/>
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
     </row>
     <row r="4" spans="2:22" ht="12.75" customHeight="1" thickBot="1">
-      <c r="E4" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="83"/>
+      <c r="E4" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="82" t="s">
+        <v>123</v>
+      </c>
+      <c r="P4" s="82"/>
       <c r="Q4" s="12"/>
       <c r="S4" s="18"/>
       <c r="T4" s="19"/>
@@ -2379,18 +2417,18 @@
     <row r="5" spans="2:22">
       <c r="B5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="85"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="84"/>
       <c r="Q5" s="20"/>
       <c r="S5" s="18"/>
       <c r="T5" s="19"/>
@@ -2398,18 +2436,18 @@
     </row>
     <row r="6" spans="2:22" s="21" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
       <c r="C6" s="22"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="87"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="86"/>
       <c r="Q6" s="23"/>
       <c r="S6" s="24"/>
       <c r="T6" s="24"/>
@@ -2418,64 +2456,64 @@
     </row>
     <row r="7" spans="2:22" s="31" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="B7" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="I7" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="L7" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="N7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="Q7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="N7" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q7" s="28" t="s">
+      <c r="R7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="R7" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="S7" s="28" t="s">
+      <c r="T7" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" s="30" t="s">
         <v>15</v>
-      </c>
-      <c r="T7" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="U7" s="30" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:22" s="39" customFormat="1" ht="40.5">
@@ -2484,343 +2522,399 @@
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="51" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K8" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>117</v>
+      </c>
       <c r="L8" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M8" s="36" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N8" s="35"/>
       <c r="O8" s="34"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="36"/>
+      <c r="P8" s="37">
+        <v>43868</v>
+      </c>
+      <c r="Q8" s="37">
+        <v>44008</v>
+      </c>
       <c r="R8" s="36"/>
       <c r="S8" s="36"/>
       <c r="T8" s="38"/>
-      <c r="U8" s="36" t="s">
-        <v>0</v>
+      <c r="U8" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="2:22" s="39" customFormat="1" ht="25.5">
       <c r="B9" s="56"/>
       <c r="C9" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>70</v>
       </c>
       <c r="F9" s="58" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H9" s="58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="59" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K9" s="58"/>
+        <v>81</v>
+      </c>
+      <c r="K9" s="58" t="s">
+        <v>117</v>
+      </c>
       <c r="L9" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M9" s="58" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N9" s="57"/>
       <c r="O9" s="60"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="58"/>
+      <c r="P9" s="37">
+        <v>43868</v>
+      </c>
+      <c r="Q9" s="37">
+        <v>44008</v>
+      </c>
       <c r="R9" s="58"/>
       <c r="S9" s="58"/>
       <c r="T9" s="60"/>
-      <c r="U9" s="58"/>
+      <c r="U9" s="58" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="10" spans="2:22" s="39" customFormat="1" ht="25.5">
       <c r="B10" s="56"/>
       <c r="C10" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="58" t="s">
-        <v>75</v>
-      </c>
       <c r="G10" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H10" s="58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="59" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="58"/>
+        <v>81</v>
+      </c>
+      <c r="K10" s="58" t="s">
+        <v>117</v>
+      </c>
       <c r="L10" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M10" s="58" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N10" s="57"/>
       <c r="O10" s="60"/>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="58"/>
+      <c r="P10" s="37">
+        <v>43868</v>
+      </c>
+      <c r="Q10" s="37">
+        <v>44008</v>
+      </c>
       <c r="R10" s="58"/>
       <c r="S10" s="58"/>
       <c r="T10" s="60"/>
-      <c r="U10" s="58"/>
-    </row>
-    <row r="11" spans="2:22" s="39" customFormat="1" ht="40.5">
+      <c r="U10" s="58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" s="39" customFormat="1" ht="54">
       <c r="B11" s="40">
         <v>2</v>
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="51" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>118</v>
+      </c>
       <c r="L11" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M11" s="36" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N11" s="35"/>
       <c r="O11" s="34"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="36"/>
+      <c r="P11" s="37">
+        <v>43903</v>
+      </c>
+      <c r="Q11" s="37">
+        <v>44008</v>
+      </c>
       <c r="R11" s="36"/>
       <c r="S11" s="36"/>
       <c r="T11" s="38"/>
-      <c r="U11" s="36"/>
+      <c r="U11" s="58" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="12" spans="2:22" s="39" customFormat="1" ht="27">
       <c r="B12" s="40"/>
       <c r="C12" s="41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>118</v>
+      </c>
       <c r="L12" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M12" s="36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="N12" s="35"/>
       <c r="O12" s="34"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="36"/>
+      <c r="P12" s="37">
+        <v>43903</v>
+      </c>
+      <c r="Q12" s="37">
+        <v>44008</v>
+      </c>
       <c r="R12" s="36"/>
       <c r="S12" s="36"/>
       <c r="T12" s="38"/>
-      <c r="U12" s="36" t="s">
-        <v>0</v>
+      <c r="U12" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="2:22" s="39" customFormat="1" ht="27">
       <c r="B13" s="40"/>
       <c r="C13" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K13" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="L13" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M13" s="36" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N13" s="35"/>
       <c r="O13" s="34"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="36"/>
+      <c r="P13" s="37">
+        <v>43903</v>
+      </c>
+      <c r="Q13" s="37">
+        <v>44008</v>
+      </c>
       <c r="R13" s="36"/>
       <c r="S13" s="36"/>
       <c r="T13" s="38"/>
-      <c r="U13" s="36" t="s">
-        <v>0</v>
+      <c r="U13" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="2:22" s="39" customFormat="1" ht="27">
       <c r="B14" s="40"/>
       <c r="C14" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K14" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K14" s="36" t="s">
+        <v>117</v>
+      </c>
       <c r="L14" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M14" s="36" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N14" s="35"/>
       <c r="O14" s="34"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="36"/>
+      <c r="P14" s="37">
+        <v>43903</v>
+      </c>
+      <c r="Q14" s="37">
+        <v>44008</v>
+      </c>
       <c r="R14" s="36"/>
       <c r="S14" s="36"/>
       <c r="T14" s="38"/>
-      <c r="U14" s="36" t="s">
-        <v>0</v>
+      <c r="U14" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="2:22" s="39" customFormat="1" ht="27">
       <c r="B15" s="40"/>
       <c r="C15" s="41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K15" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K15" s="36" t="s">
+        <v>119</v>
+      </c>
       <c r="L15" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M15" s="36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="N15" s="35"/>
       <c r="O15" s="34"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="36"/>
+      <c r="P15" s="37">
+        <v>43903</v>
+      </c>
+      <c r="Q15" s="37">
+        <v>44008</v>
+      </c>
       <c r="R15" s="36"/>
       <c r="S15" s="36"/>
       <c r="T15" s="34"/>
-      <c r="U15" s="36"/>
+      <c r="U15" s="58" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="16" spans="2:22" s="39" customFormat="1" ht="40.5">
       <c r="B16" s="40">
@@ -2828,214 +2922,248 @@
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="53" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I16" s="42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K16" s="36" t="s">
+        <v>120</v>
+      </c>
       <c r="L16" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M16" s="36" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N16" s="35"/>
       <c r="O16" s="34"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="36"/>
+      <c r="P16" s="37">
+        <v>43889</v>
+      </c>
+      <c r="Q16" s="37">
+        <v>44008</v>
+      </c>
       <c r="R16" s="36"/>
       <c r="S16" s="36"/>
       <c r="T16" s="34"/>
-      <c r="U16" s="36"/>
+      <c r="U16" s="58" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="17" spans="2:21" s="39" customFormat="1" ht="54">
       <c r="B17" s="40"/>
       <c r="C17" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="52" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H17" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K17" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K17" s="36" t="s">
+        <v>120</v>
+      </c>
       <c r="L17" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M17" s="36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N17" s="35"/>
       <c r="O17" s="34"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="36"/>
+      <c r="P17" s="37">
+        <v>43875</v>
+      </c>
+      <c r="Q17" s="37">
+        <v>44008</v>
+      </c>
       <c r="R17" s="36"/>
       <c r="S17" s="36"/>
       <c r="T17" s="34"/>
-      <c r="U17" s="36"/>
+      <c r="U17" s="58" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="18" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B18" s="40"/>
       <c r="C18" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="52" t="s">
-        <v>64</v>
-      </c>
       <c r="F18" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H18" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K18" s="36" t="s">
+        <v>120</v>
+      </c>
       <c r="L18" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M18" s="36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N18" s="35"/>
       <c r="O18" s="34"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="36"/>
+      <c r="P18" s="37">
+        <v>43868</v>
+      </c>
+      <c r="Q18" s="37">
+        <v>44008</v>
+      </c>
       <c r="R18" s="36"/>
       <c r="S18" s="36"/>
       <c r="T18" s="38"/>
-      <c r="U18" s="36" t="s">
-        <v>0</v>
+      <c r="U18" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B19" s="40"/>
       <c r="C19" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="52" t="s">
-        <v>65</v>
-      </c>
       <c r="F19" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G19" s="36" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H19" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J19" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K19" s="36" t="s">
+        <v>120</v>
+      </c>
       <c r="L19" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M19" s="36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N19" s="35"/>
       <c r="O19" s="34"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="36"/>
+      <c r="P19" s="37">
+        <v>43868</v>
+      </c>
+      <c r="Q19" s="37">
+        <v>44008</v>
+      </c>
       <c r="R19" s="36"/>
       <c r="S19" s="36"/>
       <c r="T19" s="38"/>
-      <c r="U19" s="36" t="s">
-        <v>0</v>
+      <c r="U19" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B20" s="40"/>
       <c r="C20" s="41" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D20" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="52" t="s">
-        <v>83</v>
-      </c>
       <c r="F20" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H20" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I20" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J20" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K20" s="36" t="s">
+        <v>120</v>
+      </c>
       <c r="L20" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M20" s="36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N20" s="35"/>
       <c r="O20" s="34"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="36"/>
+      <c r="P20" s="37">
+        <v>43868</v>
+      </c>
+      <c r="Q20" s="37">
+        <v>44008</v>
+      </c>
       <c r="R20" s="36"/>
       <c r="S20" s="36"/>
       <c r="T20" s="38"/>
-      <c r="U20" s="36" t="s">
-        <v>0</v>
+      <c r="U20" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="2:21" s="39" customFormat="1" ht="15.75">
@@ -3044,82 +3172,92 @@
       </c>
       <c r="C21" s="41"/>
       <c r="D21" s="51" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E21" s="52"/>
       <c r="F21" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H21" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K21" s="36"/>
       <c r="L21" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M21" s="36"/>
       <c r="N21" s="35"/>
       <c r="O21" s="34"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="36"/>
+      <c r="P21" s="37">
+        <v>43868</v>
+      </c>
+      <c r="Q21" s="37">
+        <v>44008</v>
+      </c>
       <c r="R21" s="36"/>
       <c r="S21" s="36"/>
       <c r="T21" s="38"/>
-      <c r="U21" s="36" t="s">
-        <v>0</v>
+      <c r="U21" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B22" s="40"/>
       <c r="C22" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K22" s="36"/>
+      <c r="K22" s="36" t="s">
+        <v>121</v>
+      </c>
       <c r="L22" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M22" s="36" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="N22" s="35"/>
       <c r="O22" s="34"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="36"/>
+      <c r="P22" s="37">
+        <v>43868</v>
+      </c>
+      <c r="Q22" s="37">
+        <v>44008</v>
+      </c>
       <c r="R22" s="36"/>
       <c r="S22" s="36"/>
       <c r="T22" s="38"/>
-      <c r="U22" s="36" t="s">
-        <v>0</v>
+      <c r="U22" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="2:21" s="39" customFormat="1" ht="27">
@@ -3128,82 +3266,94 @@
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="51" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E23" s="52"/>
       <c r="F23" s="36" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H23" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K23" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K23" s="36" t="s">
+        <v>121</v>
+      </c>
       <c r="L23" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M23" s="36"/>
       <c r="N23" s="35"/>
       <c r="O23" s="34"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="36"/>
+      <c r="P23" s="37">
+        <v>43959</v>
+      </c>
+      <c r="Q23" s="37">
+        <v>44008</v>
+      </c>
       <c r="R23" s="36"/>
       <c r="S23" s="36"/>
       <c r="T23" s="38"/>
-      <c r="U23" s="36" t="s">
-        <v>0</v>
+      <c r="U23" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B24" s="40"/>
       <c r="C24" s="41" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F24" s="36" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H24" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K24" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K24" s="36" t="s">
+        <v>121</v>
+      </c>
       <c r="L24" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M24" s="36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N24" s="35"/>
       <c r="O24" s="34"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="36"/>
+      <c r="P24" s="37">
+        <v>43959</v>
+      </c>
+      <c r="Q24" s="37">
+        <v>44008</v>
+      </c>
       <c r="R24" s="36"/>
       <c r="S24" s="36"/>
       <c r="T24" s="38"/>
-      <c r="U24" s="36" t="s">
-        <v>0</v>
+      <c r="U24" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="2:21" s="39" customFormat="1" ht="40.5">
@@ -3212,204 +3362,248 @@
       </c>
       <c r="C25" s="41"/>
       <c r="D25" s="51" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E25" s="52"/>
       <c r="F25" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G25" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H25" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I25" s="36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J25" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K25" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K25" s="36" t="s">
+        <v>117</v>
+      </c>
       <c r="L25" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M25" s="36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N25" s="35"/>
       <c r="O25" s="34"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="36"/>
+      <c r="P25" s="37">
+        <v>43938</v>
+      </c>
+      <c r="Q25" s="37">
+        <v>44008</v>
+      </c>
       <c r="R25" s="36"/>
       <c r="S25" s="36"/>
       <c r="T25" s="38"/>
-      <c r="U25" s="36" t="s">
-        <v>0</v>
+      <c r="U25" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B26" s="40"/>
       <c r="C26" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="52" t="s">
-        <v>94</v>
-      </c>
       <c r="F26" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H26" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J26" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K26" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K26" s="36" t="s">
+        <v>117</v>
+      </c>
       <c r="L26" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M26" s="36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N26" s="35"/>
       <c r="O26" s="34"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="36"/>
+      <c r="P26" s="37">
+        <v>43938</v>
+      </c>
+      <c r="Q26" s="37">
+        <v>44008</v>
+      </c>
       <c r="R26" s="36"/>
       <c r="S26" s="36"/>
       <c r="T26" s="38"/>
-      <c r="U26" s="36" t="s">
-        <v>0</v>
+      <c r="U26" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="2:21" s="39" customFormat="1" ht="27">
       <c r="B27" s="40"/>
       <c r="C27" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="52" t="s">
-        <v>95</v>
-      </c>
       <c r="F27" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G27" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H27" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J27" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K27" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K27" s="36" t="s">
+        <v>120</v>
+      </c>
       <c r="L27" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M27" s="36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N27" s="35"/>
       <c r="O27" s="34"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="36"/>
+      <c r="P27" s="37">
+        <v>43938</v>
+      </c>
+      <c r="Q27" s="37">
+        <v>44008</v>
+      </c>
       <c r="R27" s="36"/>
       <c r="S27" s="36"/>
       <c r="T27" s="38"/>
-      <c r="U27" s="36" t="s">
-        <v>0</v>
+      <c r="U27" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B28" s="40"/>
       <c r="C28" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="52" t="s">
-        <v>96</v>
-      </c>
       <c r="F28" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G28" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H28" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J28" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K28" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="K28" s="36" t="s">
+        <v>117</v>
+      </c>
       <c r="L28" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M28" s="36" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N28" s="35"/>
       <c r="O28" s="34"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="36"/>
+      <c r="P28" s="37">
+        <v>43938</v>
+      </c>
+      <c r="Q28" s="37">
+        <v>44008</v>
+      </c>
       <c r="R28" s="36"/>
       <c r="S28" s="36"/>
       <c r="T28" s="38"/>
-      <c r="U28" s="36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21" s="39" customFormat="1" ht="15.75">
+      <c r="U28" s="58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" s="39" customFormat="1" ht="40.5">
       <c r="B29" s="40">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C29" s="41"/>
-      <c r="D29" s="51"/>
+      <c r="D29" s="51" t="s">
+        <v>126</v>
+      </c>
       <c r="E29" s="52"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
+      <c r="F29" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="K29" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="L29" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="M29" s="36" t="s">
+        <v>125</v>
+      </c>
       <c r="N29" s="35"/>
       <c r="O29" s="34"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="36"/>
+      <c r="P29" s="37">
+        <v>43952</v>
+      </c>
+      <c r="Q29" s="37">
+        <v>44008</v>
+      </c>
       <c r="R29" s="36"/>
       <c r="S29" s="36"/>
       <c r="T29" s="38"/>
       <c r="U29" s="36" t="s">
-        <v>0</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="2:21" s="39" customFormat="1" ht="15.75">
-      <c r="B30" s="40">
-        <v>15</v>
-      </c>
+      <c r="B30" s="40"/>
       <c r="C30" s="41"/>
       <c r="D30" s="51"/>
       <c r="E30" s="52"/>
@@ -3428,9 +3622,7 @@
       <c r="R30" s="36"/>
       <c r="S30" s="36"/>
       <c r="T30" s="38"/>
-      <c r="U30" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U30" s="36"/>
     </row>
     <row r="31" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B31" s="40">
@@ -3454,9 +3646,7 @@
       <c r="R31" s="36"/>
       <c r="S31" s="36"/>
       <c r="T31" s="38"/>
-      <c r="U31" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U31" s="36"/>
     </row>
     <row r="32" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B32" s="40">
@@ -3480,9 +3670,7 @@
       <c r="R32" s="36"/>
       <c r="S32" s="36"/>
       <c r="T32" s="38"/>
-      <c r="U32" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U32" s="36"/>
     </row>
     <row r="33" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B33" s="40">
@@ -3506,9 +3694,7 @@
       <c r="R33" s="36"/>
       <c r="S33" s="36"/>
       <c r="T33" s="38"/>
-      <c r="U33" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U33" s="36"/>
     </row>
     <row r="34" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B34" s="40">
@@ -3532,9 +3718,7 @@
       <c r="R34" s="36"/>
       <c r="S34" s="36"/>
       <c r="T34" s="38"/>
-      <c r="U34" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U34" s="36"/>
     </row>
     <row r="35" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B35" s="40">
@@ -3558,9 +3742,7 @@
       <c r="R35" s="36"/>
       <c r="S35" s="36"/>
       <c r="T35" s="38"/>
-      <c r="U35" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U35" s="36"/>
     </row>
     <row r="36" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B36" s="40">
@@ -3584,9 +3766,7 @@
       <c r="R36" s="36"/>
       <c r="S36" s="36"/>
       <c r="T36" s="38"/>
-      <c r="U36" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U36" s="36"/>
     </row>
     <row r="37" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B37" s="40">
@@ -3610,9 +3790,7 @@
       <c r="R37" s="36"/>
       <c r="S37" s="36"/>
       <c r="T37" s="38"/>
-      <c r="U37" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U37" s="36"/>
     </row>
     <row r="38" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B38" s="40">
@@ -3636,9 +3814,7 @@
       <c r="R38" s="36"/>
       <c r="S38" s="36"/>
       <c r="T38" s="38"/>
-      <c r="U38" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U38" s="36"/>
     </row>
     <row r="39" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B39" s="40">
@@ -3662,9 +3838,7 @@
       <c r="R39" s="36"/>
       <c r="S39" s="36"/>
       <c r="T39" s="38"/>
-      <c r="U39" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U39" s="36"/>
     </row>
     <row r="40" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B40" s="40">
@@ -3688,9 +3862,7 @@
       <c r="R40" s="36"/>
       <c r="S40" s="36"/>
       <c r="T40" s="38"/>
-      <c r="U40" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U40" s="36"/>
     </row>
     <row r="41" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B41" s="40">
@@ -3714,9 +3886,7 @@
       <c r="R41" s="36"/>
       <c r="S41" s="36"/>
       <c r="T41" s="38"/>
-      <c r="U41" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U41" s="36"/>
     </row>
     <row r="42" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B42" s="40">
@@ -3740,9 +3910,7 @@
       <c r="R42" s="36"/>
       <c r="S42" s="36"/>
       <c r="T42" s="38"/>
-      <c r="U42" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U42" s="36"/>
     </row>
     <row r="43" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B43" s="40">
@@ -3766,9 +3934,7 @@
       <c r="R43" s="36"/>
       <c r="S43" s="36"/>
       <c r="T43" s="38"/>
-      <c r="U43" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U43" s="36"/>
     </row>
     <row r="44" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B44" s="40">
@@ -3792,9 +3958,7 @@
       <c r="R44" s="36"/>
       <c r="S44" s="36"/>
       <c r="T44" s="38"/>
-      <c r="U44" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U44" s="36"/>
     </row>
     <row r="45" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B45" s="40">
@@ -3818,9 +3982,7 @@
       <c r="R45" s="36"/>
       <c r="S45" s="36"/>
       <c r="T45" s="38"/>
-      <c r="U45" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U45" s="36"/>
     </row>
     <row r="46" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B46" s="40">
@@ -3844,9 +4006,7 @@
       <c r="R46" s="36"/>
       <c r="S46" s="36"/>
       <c r="T46" s="38"/>
-      <c r="U46" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U46" s="36"/>
     </row>
     <row r="47" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B47" s="40">
@@ -3870,9 +4030,7 @@
       <c r="R47" s="36"/>
       <c r="S47" s="36"/>
       <c r="T47" s="38"/>
-      <c r="U47" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U47" s="36"/>
     </row>
     <row r="48" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B48" s="40">
@@ -3896,9 +4054,7 @@
       <c r="R48" s="36"/>
       <c r="S48" s="36"/>
       <c r="T48" s="38"/>
-      <c r="U48" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U48" s="36"/>
     </row>
     <row r="49" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B49" s="40">
@@ -3922,9 +4078,7 @@
       <c r="R49" s="36"/>
       <c r="S49" s="36"/>
       <c r="T49" s="38"/>
-      <c r="U49" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U49" s="36"/>
     </row>
     <row r="50" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B50" s="40">
@@ -3948,9 +4102,7 @@
       <c r="R50" s="36"/>
       <c r="S50" s="36"/>
       <c r="T50" s="38"/>
-      <c r="U50" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U50" s="36"/>
     </row>
     <row r="51" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B51" s="40">
@@ -3974,9 +4126,7 @@
       <c r="R51" s="36"/>
       <c r="S51" s="36"/>
       <c r="T51" s="38"/>
-      <c r="U51" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U51" s="36"/>
     </row>
     <row r="52" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B52" s="40">
@@ -4000,9 +4150,7 @@
       <c r="R52" s="36"/>
       <c r="S52" s="36"/>
       <c r="T52" s="38"/>
-      <c r="U52" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U52" s="36"/>
     </row>
     <row r="53" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B53" s="40">
@@ -4026,9 +4174,7 @@
       <c r="R53" s="36"/>
       <c r="S53" s="36"/>
       <c r="T53" s="38"/>
-      <c r="U53" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U53" s="36"/>
     </row>
     <row r="54" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B54" s="40">
@@ -4052,9 +4198,7 @@
       <c r="R54" s="36"/>
       <c r="S54" s="36"/>
       <c r="T54" s="38"/>
-      <c r="U54" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U54" s="36"/>
     </row>
     <row r="55" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B55" s="40">
@@ -4078,9 +4222,7 @@
       <c r="R55" s="36"/>
       <c r="S55" s="36"/>
       <c r="T55" s="38"/>
-      <c r="U55" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U55" s="36"/>
     </row>
     <row r="56" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B56" s="40">
@@ -4104,9 +4246,7 @@
       <c r="R56" s="36"/>
       <c r="S56" s="36"/>
       <c r="T56" s="38"/>
-      <c r="U56" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U56" s="36"/>
     </row>
     <row r="57" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B57" s="40">
@@ -4130,9 +4270,7 @@
       <c r="R57" s="36"/>
       <c r="S57" s="36"/>
       <c r="T57" s="38"/>
-      <c r="U57" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U57" s="36"/>
     </row>
     <row r="58" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B58" s="40">
@@ -4156,9 +4294,7 @@
       <c r="R58" s="36"/>
       <c r="S58" s="36"/>
       <c r="T58" s="38"/>
-      <c r="U58" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U58" s="36"/>
     </row>
     <row r="59" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B59" s="40">
@@ -4182,9 +4318,7 @@
       <c r="R59" s="36"/>
       <c r="S59" s="36"/>
       <c r="T59" s="38"/>
-      <c r="U59" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U59" s="36"/>
     </row>
     <row r="60" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B60" s="40">
@@ -4208,9 +4342,7 @@
       <c r="R60" s="36"/>
       <c r="S60" s="36"/>
       <c r="T60" s="38"/>
-      <c r="U60" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U60" s="36"/>
     </row>
     <row r="61" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B61" s="40">
@@ -4234,9 +4366,7 @@
       <c r="R61" s="36"/>
       <c r="S61" s="36"/>
       <c r="T61" s="38"/>
-      <c r="U61" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U61" s="36"/>
     </row>
     <row r="62" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B62" s="40">
@@ -4260,9 +4390,7 @@
       <c r="R62" s="36"/>
       <c r="S62" s="36"/>
       <c r="T62" s="38"/>
-      <c r="U62" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U62" s="36"/>
     </row>
     <row r="63" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B63" s="40">
@@ -4286,9 +4414,7 @@
       <c r="R63" s="36"/>
       <c r="S63" s="36"/>
       <c r="T63" s="38"/>
-      <c r="U63" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U63" s="36"/>
     </row>
     <row r="64" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B64" s="40">
@@ -4312,9 +4438,7 @@
       <c r="R64" s="36"/>
       <c r="S64" s="36"/>
       <c r="T64" s="38"/>
-      <c r="U64" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U64" s="36"/>
     </row>
     <row r="65" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B65" s="40">
@@ -4338,9 +4462,7 @@
       <c r="R65" s="36"/>
       <c r="S65" s="36"/>
       <c r="T65" s="38"/>
-      <c r="U65" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U65" s="36"/>
     </row>
     <row r="66" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B66" s="40">
@@ -4364,9 +4486,7 @@
       <c r="R66" s="36"/>
       <c r="S66" s="36"/>
       <c r="T66" s="38"/>
-      <c r="U66" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U66" s="36"/>
     </row>
     <row r="67" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B67" s="40">
@@ -4390,9 +4510,7 @@
       <c r="R67" s="36"/>
       <c r="S67" s="36"/>
       <c r="T67" s="38"/>
-      <c r="U67" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U67" s="36"/>
     </row>
     <row r="68" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B68" s="40">
@@ -4416,9 +4534,7 @@
       <c r="R68" s="36"/>
       <c r="S68" s="36"/>
       <c r="T68" s="38"/>
-      <c r="U68" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U68" s="36"/>
     </row>
     <row r="69" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B69" s="40">
@@ -4442,9 +4558,7 @@
       <c r="R69" s="36"/>
       <c r="S69" s="36"/>
       <c r="T69" s="38"/>
-      <c r="U69" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U69" s="36"/>
     </row>
     <row r="70" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B70" s="40">
@@ -4468,9 +4582,7 @@
       <c r="R70" s="36"/>
       <c r="S70" s="36"/>
       <c r="T70" s="38"/>
-      <c r="U70" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U70" s="36"/>
     </row>
     <row r="71" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B71" s="40">
@@ -4494,9 +4606,7 @@
       <c r="R71" s="36"/>
       <c r="S71" s="36"/>
       <c r="T71" s="38"/>
-      <c r="U71" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U71" s="36"/>
     </row>
     <row r="72" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B72" s="40">
@@ -4520,9 +4630,7 @@
       <c r="R72" s="36"/>
       <c r="S72" s="36"/>
       <c r="T72" s="38"/>
-      <c r="U72" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U72" s="36"/>
     </row>
     <row r="73" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B73" s="40">
@@ -4546,9 +4654,7 @@
       <c r="R73" s="36"/>
       <c r="S73" s="36"/>
       <c r="T73" s="38"/>
-      <c r="U73" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U73" s="36"/>
     </row>
     <row r="74" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B74" s="40">
@@ -4572,9 +4678,7 @@
       <c r="R74" s="36"/>
       <c r="S74" s="36"/>
       <c r="T74" s="38"/>
-      <c r="U74" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U74" s="36"/>
     </row>
     <row r="75" spans="2:21" s="39" customFormat="1" ht="15.75">
       <c r="B75" s="40">
@@ -4598,9 +4702,7 @@
       <c r="R75" s="36"/>
       <c r="S75" s="36"/>
       <c r="T75" s="38"/>
-      <c r="U75" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U75" s="36"/>
     </row>
     <row r="76" spans="2:21" s="39" customFormat="1" ht="16.5" thickBot="1">
       <c r="B76" s="43">
@@ -4624,9 +4726,7 @@
       <c r="R76" s="47"/>
       <c r="S76" s="47"/>
       <c r="T76" s="49"/>
-      <c r="U76" s="36" t="s">
-        <v>0</v>
-      </c>
+      <c r="U76" s="36"/>
     </row>
     <row r="77" spans="2:21">
       <c r="N77" s="12"/>

</xml_diff>